<commit_message>
added notes to Effort Estimation
</commit_message>
<xml_diff>
--- a/01_ProjectPlanning/06_EffortEstimation.xlsx
+++ b/01_ProjectPlanning/06_EffortEstimation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lindi\.aSchule\3CHIF\SYP\Projekt_ADL\01_ProjectPlanning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77D9384-89E2-4031-A9ED-605B73D181B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3833260-045F-4664-A589-C2F4576A7596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5820" yWindow="1830" windowWidth="18000" windowHeight="10950" xr2:uid="{FFCB8E78-0403-4EBC-A114-9EF481813729}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="18000" windowHeight="10950" xr2:uid="{FFCB8E78-0403-4EBC-A114-9EF481813729}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>Task</t>
   </si>
@@ -97,6 +97,18 @@
   </si>
   <si>
     <t>6 Hours</t>
+  </si>
+  <si>
+    <t>Mehr darauf achten Zeit nicht zu unterschätzen!</t>
+  </si>
+  <si>
+    <t>Effort von allen 3 Mitgliedern beachten!</t>
+  </si>
+  <si>
+    <t>Bessere Aufteilung der Aufgaben</t>
+  </si>
+  <si>
+    <t>Notes:</t>
   </si>
 </sst>
 </file>
@@ -465,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{212A95A6-4E6B-43AC-808A-DB8CE0B9DFB7}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,6 +569,26 @@
         <v>14</v>
       </c>
     </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added notes to EffortEstimation
</commit_message>
<xml_diff>
--- a/01_ProjectPlanning/06_EffortEstimation.xlsx
+++ b/01_ProjectPlanning/06_EffortEstimation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lindi\.aSchule\3CHIF\SYP\Projekt_ADL\01_ProjectPlanning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3833260-045F-4664-A589-C2F4576A7596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC3AAFC3-75F6-44D7-A328-201EF9D56CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1125" yWindow="1125" windowWidth="18000" windowHeight="10950" xr2:uid="{FFCB8E78-0403-4EBC-A114-9EF481813729}"/>
   </bookViews>
@@ -158,10 +158,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="60 % - Akzent1" xfId="1" builtinId="32"/>
@@ -477,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{212A95A6-4E6B-43AC-808A-DB8CE0B9DFB7}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,17 +576,22 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>21</v>
+      <c r="A7" s="3">
+        <v>44610</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>